<commit_message>
Update with source murine CEDAR docs - #52
</commit_message>
<xml_diff>
--- a/docs/libraries/ingest-validation-tools/schemas/source-murine/murine-source.xlsx
+++ b/docs/libraries/ingest-validation-tools/schemas/source-murine/murine-source.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LIB118/Work/sennetdocs/docs/libraries/ingest-validation-tools/schemas/source-murine/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E82F7B-7D11-EA46-95DC-08C530032856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="28640" windowHeight="11000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
@@ -16,17 +22,17 @@
     <sheet name="bedding list" sheetId="7" r:id="rId7"/>
     <sheet name="cage_enhancements list" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -39,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -78,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -91,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -117,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -130,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -143,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -156,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -169,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -182,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -195,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -208,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -221,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -234,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -247,16 +253,30 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t>Environmental enrichments present in the source’s cage.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{4DCE23A1-F1BA-C846-834F-644295C377D9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The string that serves as the definitive identifier for the metadata schema version.</t>
         </r>
       </text>
     </comment>
@@ -265,7 +285,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>source_id</t>
   </si>
@@ -418,13 +438,16 @@
   </si>
   <si>
     <t>Nylon bones</t>
+  </si>
+  <si>
+    <t>metadata_schema_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,6 +468,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -478,13 +514,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -522,7 +566,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -556,6 +600,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -590,9 +635,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -765,17 +811,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -830,60 +876,87 @@
       <c r="R1" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: M / F." sqref="D2:D1048576">
-      <formula1>'sex list'!$A$1:$A$2</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="E2:E1048576">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="E2:E1048576 G2:G1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="G2:G1048576">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from euthanization_method list." sqref="I2:I1048576">
-      <formula1>'euthanization_method list'!$A$1:$A$8</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Pathogen free / Pathogen and opportunist free / Other." sqref="K2:K1048576">
-      <formula1>'room_health_status list'!$A$1:$A$3</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="L2:L1048576">
-      <formula1>-1e+307</formula1>
-      <formula2>1e+307</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Biocontainment / Ventilated / Micro-Isolator / Conventional." sqref="M2:M1048576">
-      <formula1>'rack_setup list'!$A$1:$A$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Standard/default / Longer photoperiods / Reverse light cycles." sqref="N2:N1048576">
-      <formula1>'light_cycle list'!$A$1:$A$3</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from bedding list." sqref="O2:O1048576">
-      <formula1>'bedding list'!$A$1:$A$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from cage_enhancements list." sqref="R2:R1048576">
-      <formula1>'cage_enhancements list'!$A$1:$A$6</formula1>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="L2:L1048576" xr:uid="{00000000-0002-0000-0000-000005000000}">
+      <formula1>-1E+307</formula1>
+      <formula2>1E+307</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: M / F." xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>'sex list'!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from euthanization_method list." xr:uid="{00000000-0002-0000-0000-000003000000}">
+          <x14:formula1>
+            <xm:f>'euthanization_method list'!$A$1:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Pathogen free / Pathogen and opportunist free / Other." xr:uid="{00000000-0002-0000-0000-000004000000}">
+          <x14:formula1>
+            <xm:f>'room_health_status list'!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Biocontainment / Ventilated / Micro-Isolator / Conventional." xr:uid="{00000000-0002-0000-0000-000006000000}">
+          <x14:formula1>
+            <xm:f>'rack_setup list'!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Standard/default / Longer photoperiods / Reverse light cycles." xr:uid="{00000000-0002-0000-0000-000007000000}">
+          <x14:formula1>
+            <xm:f>'light_cycle list'!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>N2:N1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from bedding list." xr:uid="{00000000-0002-0000-0000-000008000000}">
+          <x14:formula1>
+            <xm:f>'bedding list'!$A$1:$A$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:O1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from cage_enhancements list." xr:uid="{00000000-0002-0000-0000-000009000000}">
+          <x14:formula1>
+            <xm:f>'cage_enhancements list'!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>R2:R1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -894,49 +967,49 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -947,24 +1020,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -975,29 +1048,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1008,24 +1081,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1036,59 +1109,59 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1099,39 +1172,39 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>

</xml_diff>